<commit_message>
Tilføjet mapper og rykket rundt i Bilagmappen
</commit_message>
<xml_diff>
--- a/Tidsplan/Tidsplan - projekt.xlsx
+++ b/Tidsplan/Tidsplan - projekt.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -315,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -353,6 +353,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -670,7 +671,7 @@
   <dimension ref="A1:R41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+      <selection sqref="A1:R41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1235,18 +1236,18 @@
       <c r="B35" s="15"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="30"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="23"/>
-      <c r="K35" s="23"/>
-      <c r="L35" s="23"/>
-      <c r="M35" s="23"/>
-      <c r="N35" s="30"/>
-      <c r="O35" s="23"/>
-      <c r="P35" s="23"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="37"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="37"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="3"/>
       <c r="Q35" s="23"/>
       <c r="R35" s="30"/>
     </row>

</xml_diff>